<commit_message>
Preview data before import
</commit_message>
<xml_diff>
--- a/admin/planetedu.xlsx
+++ b/admin/planetedu.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\edu-bootstrap\admin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA5DC33-74D7-414F-A97E-7DC1F5596E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14295" windowHeight="5385" tabRatio="598" activeTab="4"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="598" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCHOOL" sheetId="4" r:id="rId1"/>
@@ -678,8 +684,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -769,6 +775,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -815,7 +829,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -847,9 +861,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -881,6 +913,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1056,14 +1106,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
@@ -1076,7 +1126,7 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
@@ -1105,7 +1155,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1136,21 +1186,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
@@ -1160,7 +1210,7 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
@@ -1183,7 +1233,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1206,7 +1256,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1231,24 +1281,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
@@ -1260,7 +1310,7 @@
       </c>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1293,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1315,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1326,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1337,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1348,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1370,7 +1420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1403,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1414,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1425,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1436,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1458,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1469,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1480,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1491,7 +1541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1502,7 +1552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1513,7 +1563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1524,7 +1574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1535,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1546,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1557,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1568,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1601,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1612,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1623,7 +1673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1634,7 +1684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1645,7 +1695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1662,14 +1712,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -1682,7 +1732,7 @@
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>85</v>
       </c>
@@ -1714,7 +1764,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1111111</v>
       </c>
@@ -1741,7 +1791,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1111112</v>
       </c>
@@ -1768,7 +1818,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1111113</v>
       </c>
@@ -1795,7 +1845,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1111114</v>
       </c>
@@ -1822,7 +1872,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1111115</v>
       </c>
@@ -1849,7 +1899,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1111116</v>
       </c>
@@ -1876,7 +1926,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1111117</v>
       </c>
@@ -1903,7 +1953,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1111118</v>
       </c>
@@ -1930,7 +1980,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1111119</v>
       </c>
@@ -1957,7 +2007,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1111120</v>
       </c>
@@ -1984,7 +2034,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1111121</v>
       </c>
@@ -2011,7 +2061,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1111122</v>
       </c>
@@ -2038,7 +2088,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1111123</v>
       </c>
@@ -2065,7 +2115,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1111124</v>
       </c>
@@ -2092,7 +2142,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1111125</v>
       </c>
@@ -2119,7 +2169,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1111126</v>
       </c>
@@ -2146,7 +2196,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1111127</v>
       </c>
@@ -2173,7 +2223,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1111128</v>
       </c>
@@ -2200,7 +2250,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1111129</v>
       </c>
@@ -2227,7 +2277,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1111130</v>
       </c>
@@ -2254,7 +2304,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1111131</v>
       </c>
@@ -2281,7 +2331,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1111132</v>
       </c>
@@ -2308,7 +2358,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1111133</v>
       </c>
@@ -2335,7 +2385,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1111134</v>
       </c>
@@ -2362,7 +2412,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1111135</v>
       </c>
@@ -2388,7 +2438,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1111136</v>
       </c>
@@ -2414,7 +2464,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1111137</v>
       </c>
@@ -2440,7 +2490,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1111138</v>
       </c>
@@ -2466,7 +2516,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1111139</v>
       </c>
@@ -2492,7 +2542,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1111140</v>
       </c>
@@ -2518,7 +2568,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1111141</v>
       </c>
@@ -2550,14 +2600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -2568,7 +2618,7 @@
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>85</v>
       </c>
@@ -2597,7 +2647,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001001001</v>
       </c>
@@ -2621,7 +2671,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10001001002</v>
       </c>
@@ -2645,7 +2695,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10001001003</v>
       </c>
@@ -2669,7 +2719,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10001001004</v>
       </c>
@@ -2693,7 +2743,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10001001005</v>
       </c>
@@ -2717,7 +2767,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10001001006</v>
       </c>
@@ -2741,7 +2791,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10001001007</v>
       </c>
@@ -2765,7 +2815,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10001001008</v>
       </c>
@@ -2789,7 +2839,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10001001009</v>
       </c>
@@ -2813,7 +2863,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10001001010</v>
       </c>
@@ -2837,7 +2887,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10001001011</v>
       </c>
@@ -2861,7 +2911,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10001001012</v>
       </c>
@@ -2885,7 +2935,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10001001013</v>
       </c>
@@ -2909,7 +2959,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10001001014</v>
       </c>
@@ -2933,7 +2983,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10001001015</v>
       </c>
@@ -2957,7 +3007,7 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10001001016</v>
       </c>
@@ -2981,7 +3031,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10001001017</v>
       </c>
@@ -3005,7 +3055,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10001001018</v>
       </c>
@@ -3029,7 +3079,7 @@
       </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10001001019</v>
       </c>
@@ -3053,7 +3103,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10001001020</v>
       </c>
@@ -3077,7 +3127,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10001001021</v>
       </c>
@@ -3101,7 +3151,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10001001022</v>
       </c>
@@ -3125,7 +3175,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10001001023</v>
       </c>
@@ -3156,21 +3206,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -3187,7 +3237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -3201,7 +3251,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>91</v>
       </c>
@@ -3215,7 +3265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
@@ -3232,7 +3282,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -3246,7 +3296,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>91</v>
       </c>
@@ -3260,7 +3310,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>91</v>
       </c>
@@ -3274,7 +3324,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>91</v>
       </c>
@@ -3288,7 +3338,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>91</v>
       </c>
@@ -3302,7 +3352,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
@@ -3316,7 +3366,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>87</v>
       </c>
@@ -3330,7 +3380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>87</v>
       </c>
@@ -3344,7 +3394,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>87</v>
       </c>
@@ -3358,7 +3408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3372,7 +3422,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>87</v>
       </c>
@@ -3386,7 +3436,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>87</v>
       </c>
@@ -3400,7 +3450,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -3414,7 +3464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>87</v>
       </c>
@@ -3428,7 +3478,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
@@ -3442,7 +3492,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
@@ -3456,7 +3506,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>87</v>
       </c>
@@ -3470,7 +3520,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>87</v>
       </c>
@@ -3484,7 +3534,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -3498,7 +3548,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>92</v>
       </c>
@@ -3512,7 +3562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>92</v>
       </c>
@@ -3526,7 +3576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>93</v>
       </c>
@@ -3540,7 +3590,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>93</v>
       </c>

</xml_diff>